<commit_message>
update Tagebuch von Manyue
</commit_message>
<xml_diff>
--- a/dev-diaries/diary-person-3.xlsx
+++ b/dev-diaries/diary-person-3.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friedrich\Projekte\dlvc\vorlagen\content\dev-diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\group-1\dev-diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB6532-3F41-4D28-AF69-22E3E80B3CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="38" windowWidth="15960" windowHeight="17348" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diary" sheetId="1" r:id="rId1"/>
     <sheet name="Reflection" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -49,18 +63,6 @@
     <t>Beitrag zum Projekt</t>
   </si>
   <si>
-    <t>Erste Infoveranstaltung - Einführung in das Projekt und Vorstellung der Teams sowie erste grobe Einteilung</t>
-  </si>
-  <si>
-    <t>Ablauf, Organisatorisches, Projektziel, Vorstellung der Themen</t>
-  </si>
-  <si>
-    <t>Max Muster</t>
-  </si>
-  <si>
-    <t>Gesamtzeit (bei 8 ECTS):</t>
-  </si>
-  <si>
     <t>KW 11</t>
   </si>
   <si>
@@ -74,9 +76,6 @@
   </si>
   <si>
     <t>Zeitaufwand in Dreiviertelstunden</t>
-  </si>
-  <si>
-    <t>Team X</t>
   </si>
   <si>
     <t>Team-Mitglied</t>
@@ -96,12 +95,117 @@
   <si>
     <t>w</t>
   </si>
+  <si>
+    <t>Manyue Zhang</t>
+  </si>
+  <si>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t>Gesamtzeit (bei 5 ECTS):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. wie man Captum Insight bedienen kann
+2. Kenntnisse über Captum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. rechechieren und Paper von entsprechenden Algorithmen lesen 
+2. mit den Gruppenmitgliedern über eigene Verständnis von Algorithmen diskutieren 
+3. Guided Backpagation und Deconvolution vorstellen und erklären  </t>
+  </si>
+  <si>
+    <t>1. Ablauf, Organisatorisches, Projektziel, Vorstellung der Themen.
+2. Ziele bis nächste Woche festlegen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git Repository und Wiki erstellen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. was Deconvolution ist und die Unterscheide zwischen Convolution und Deconvolution 
+2. wie die Deconvolution in Captum umgesetzt wird und die Vorteile von Deconvolution
+3. die Hauptidee von Guided Backpropagation </t>
+  </si>
+  <si>
+    <t>1. Inhalte und Aufgabenaufteilung mit Teamkollege festlegen
+2. Onenote Zusammenfassung erstellt und geteilt</t>
+  </si>
+  <si>
+    <t>28.03.2023-02.04.2023</t>
+  </si>
+  <si>
+    <t>KW 12</t>
+  </si>
+  <si>
+    <t>03.04.2023-09.04.2023</t>
+  </si>
+  <si>
+    <t>10.04.2023-16.04.2023</t>
+  </si>
+  <si>
+    <t>17.04.2023-23.04.2023</t>
+  </si>
+  <si>
+    <t>24.04.2023-30.04.2023</t>
+  </si>
+  <si>
+    <t>KW 13</t>
+  </si>
+  <si>
+    <t>KW 14</t>
+  </si>
+  <si>
+    <t>kw15</t>
+  </si>
+  <si>
+    <t>kw16</t>
+  </si>
+  <si>
+    <t>1. Vorlesung über Fortgeschrittene Architekturen und Transfer Learning</t>
+  </si>
+  <si>
+    <t>1. entsprechende Algorithmen zu jedem Mitgelieder teilen. 
+2. Entwicklungsumgegung zur GUI erstellen und teilen</t>
+  </si>
+  <si>
+    <t>1. Captum mit Streamlit weiter integieren.
+2. Paper recherchieren 
+3. für Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>paare Fachbegriffe unter Integrated Gradients wie Baseline Value, Sensitivity, Implementation Invariance, Symmmetry-Preserving versstehen</t>
+  </si>
+  <si>
+    <t>1. Vorlesung: Erste Infoveranstaltung - Einführung in das Projekt und Vorstellung der Teams sowie erste grobe Einteilung
+2.Praktikum: über unsereProjektsthema rechechieren
+3. Paper "Axiomatic Attribution for Deep Networks" lesen</t>
+  </si>
+  <si>
+    <t>1. Captum Insight zum Laufen bringen 
+2. Tutoriale Videos über Integrated Gradients schauen
+2. mit Gruppenmitgliedern darüber austauschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. verschiende Algorithmen auf Captum Insight fetchen
+2. Algorithmen zuweisen(Guided Backpagation und Deconvolution)</t>
+  </si>
+  <si>
+    <t>1. die Hälfte Demo ist fertig
+2.Fachbegriffe von Paper erklären
+3.Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>kw17</t>
+  </si>
+  <si>
+    <t>01.05.2023-07.05.2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -144,6 +248,17 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -246,82 +361,123 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="39">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +579,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -486,6 +641,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0A05-4932-9F40-7C91D4842066}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -501,6 +661,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0A05-4932-9F40-7C91D4842066}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -516,6 +681,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0A05-4932-9F40-7C91D4842066}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -531,6 +701,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-0A05-4932-9F40-7C91D4842066}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -600,7 +775,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1243,7 +1417,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2365,29 +2545,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.19921875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.19921875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="35.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.86328125" style="1" customWidth="1"/>
-    <col min="9" max="18" width="17.19921875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="17.19921875" style="1"/>
+    <col min="1" max="1" width="17.1796875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="35.81640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="40.6328125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="1" customWidth="1"/>
+    <col min="9" max="18" width="17.1796875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="17.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+    <row r="1" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2401,14 +2585,14 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2422,20 +2606,20 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="B3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="23"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -2449,16 +2633,16 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -2472,164 +2656,178 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="7" t="s">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8">
+      <c r="H6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="5">
         <f>SUM(F10:F152)</f>
-        <v>2</v>
-      </c>
-      <c r="G7" s="8">
+        <v>61</v>
+      </c>
+      <c r="G7" s="5">
         <f>H7-F7</f>
-        <v>148</v>
-      </c>
-      <c r="H7" s="8">
+        <v>89</v>
+      </c>
+      <c r="H7" s="5">
         <f>5*30</f>
         <v>150</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="11">
         <v>17</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="18">
-        <v>44475</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20">
-        <v>2</v>
-      </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-    </row>
-    <row r="11" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2">
+        <v>15</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2642,13 +2840,23 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+    <row r="12" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="13">
+        <v>16</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2661,13 +2869,25 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2">
+        <v>13</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2680,12 +2900,22 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2699,12 +2929,16 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="191.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:17" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -2718,12 +2952,14 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2737,12 +2973,12 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -2756,12 +2992,12 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+    <row r="18" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2775,12 +3011,12 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2794,12 +3030,12 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+    <row r="20" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2813,12 +3049,12 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2832,12 +3068,12 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+    <row r="22" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -2851,12 +3087,12 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -2870,12 +3106,12 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2889,12 +3125,12 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2908,12 +3144,12 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2927,12 +3163,12 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2946,12 +3182,12 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -2965,12 +3201,12 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2984,12 +3220,12 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -3003,12 +3239,12 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -3022,12 +3258,12 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3041,12 +3277,12 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -3060,12 +3296,12 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -3079,12 +3315,12 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -3098,12 +3334,12 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -3117,12 +3353,12 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -3136,12 +3372,12 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -3155,12 +3391,12 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -3174,12 +3410,12 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -3193,12 +3429,12 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -3212,12 +3448,12 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3231,12 +3467,12 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3250,12 +3486,12 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -3269,12 +3505,12 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -3288,12 +3524,12 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="31"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -3307,12 +3543,12 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3326,12 +3562,12 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -3345,12 +3581,12 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -3364,12 +3600,12 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="31"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -3383,12 +3619,12 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="31"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3402,12 +3638,12 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3421,12 +3657,12 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3440,12 +3676,12 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3459,12 +3695,12 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3478,12 +3714,12 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -3497,12 +3733,12 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3516,12 +3752,12 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3535,12 +3771,12 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3554,12 +3790,12 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3573,12 +3809,12 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="31"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3592,12 +3828,12 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="31"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3611,12 +3847,12 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3630,12 +3866,12 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="31"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -3649,12 +3885,12 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3668,12 +3904,12 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3687,12 +3923,12 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="31"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3706,12 +3942,12 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="31"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -3725,12 +3961,12 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="2"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
+    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -3744,12 +3980,12 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="2"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3763,12 +3999,12 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="2"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -3782,12 +4018,12 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="31"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -3801,12 +4037,12 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="31"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -3820,12 +4056,12 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="2"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="31"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -3839,12 +4075,12 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="31"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -3858,12 +4094,12 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="2"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
+    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="31"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -3877,12 +4113,12 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
+    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3896,12 +4132,12 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="2"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
+    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="31"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -3915,12 +4151,12 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="2"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
+    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="31"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3934,12 +4170,12 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="2"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="31"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3953,12 +4189,12 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="2"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="31"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -3972,12 +4208,12 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="31"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -3991,12 +4227,12 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="2"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -4010,12 +4246,12 @@
       <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
     </row>
-    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="2"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="31"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -4029,12 +4265,12 @@
       <c r="P84" s="2"/>
       <c r="Q84" s="2"/>
     </row>
-    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="2"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="31"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -4048,12 +4284,12 @@
       <c r="P85" s="2"/>
       <c r="Q85" s="2"/>
     </row>
-    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="2"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
+    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="31"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -4067,12 +4303,12 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
-    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="31"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -4086,12 +4322,12 @@
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="2"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="31"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -4105,12 +4341,12 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="2"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="31"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -4124,12 +4360,12 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
-    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="2"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
+    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="31"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -4143,12 +4379,12 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="2"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
+    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="31"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -4162,12 +4398,12 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="2"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
+    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -4181,12 +4417,12 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="2"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
+    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="31"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -4200,12 +4436,12 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="2"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
+    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="31"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -4219,12 +4455,12 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="2"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="31"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -4238,12 +4474,12 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="2"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
+    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="31"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -4257,12 +4493,12 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="2"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
+    <row r="97" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="31"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -4276,12 +4512,12 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="2"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
+    <row r="98" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -4295,12 +4531,12 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="2"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+    <row r="99" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="31"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -4314,12 +4550,12 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="2"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
+    <row r="100" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="31"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -4333,12 +4569,12 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="2"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -4352,12 +4588,12 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="2"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
+    <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="31"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="23"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -4371,12 +4607,12 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="2"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
+    <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="31"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="23"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
@@ -4390,12 +4626,12 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="2"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
+    <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="31"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="23"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="23"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -4409,12 +4645,12 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="2"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
+    <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="31"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -4428,12 +4664,12 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
+    <row r="106" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="31"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -4447,12 +4683,12 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
+    <row r="107" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="31"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="23"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -4466,12 +4702,12 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
+    <row r="108" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="31"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="23"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -4485,12 +4721,12 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
+    <row r="109" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="31"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -4504,12 +4740,12 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
+    <row r="110" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="31"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -4523,12 +4759,12 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
+    <row r="111" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="31"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="23"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="23"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
@@ -4542,12 +4778,12 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
+    <row r="112" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="31"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
@@ -4561,12 +4797,12 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
+    <row r="113" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="31"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -4580,12 +4816,12 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="2"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
+    <row r="114" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="31"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
@@ -4599,12 +4835,12 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
+    <row r="115" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="31"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="23"/>
+      <c r="D115" s="23"/>
+      <c r="E115" s="23"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
@@ -4618,12 +4854,12 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
+    <row r="116" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="31"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
@@ -4637,12 +4873,12 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
+    <row r="117" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="31"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="23"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="23"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
@@ -4656,12 +4892,12 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
+    <row r="118" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="31"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="23"/>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
@@ -4675,12 +4911,12 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
+    <row r="119" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="31"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="23"/>
+      <c r="D119" s="23"/>
+      <c r="E119" s="23"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
@@ -4694,12 +4930,12 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
+    <row r="120" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="31"/>
+      <c r="B120" s="18"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="23"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
@@ -4713,12 +4949,12 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
+    <row r="121" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="31"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
@@ -4732,12 +4968,12 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
+    <row r="122" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="31"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="23"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
@@ -4751,12 +4987,12 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
+    <row r="123" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
+      <c r="B123" s="18"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
@@ -4770,12 +5006,12 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
+    <row r="124" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
+      <c r="B124" s="18"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
@@ -4789,12 +5025,12 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
+    <row r="125" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
+      <c r="B125" s="18"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
@@ -4808,12 +5044,12 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
+    <row r="126" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
+      <c r="B126" s="18"/>
+      <c r="C126" s="23"/>
+      <c r="D126" s="23"/>
+      <c r="E126" s="23"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
@@ -4827,12 +5063,12 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
+    <row r="127" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
+      <c r="B127" s="18"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="23"/>
+      <c r="E127" s="23"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
@@ -4846,12 +5082,12 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
+    <row r="128" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
+      <c r="B128" s="18"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="23"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
@@ -4865,12 +5101,12 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
+    <row r="129" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="31"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="23"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
@@ -4884,12 +5120,12 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
+    <row r="130" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="31"/>
+      <c r="B130" s="18"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
@@ -4903,12 +5139,12 @@
       <c r="P130" s="2"/>
       <c r="Q130" s="2"/>
     </row>
-    <row r="131" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
+    <row r="131" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="31"/>
+      <c r="B131" s="18"/>
+      <c r="C131" s="23"/>
+      <c r="D131" s="23"/>
+      <c r="E131" s="23"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
@@ -4922,12 +5158,12 @@
       <c r="P131" s="2"/>
       <c r="Q131" s="2"/>
     </row>
-    <row r="132" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
+    <row r="132" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="31"/>
+      <c r="B132" s="18"/>
+      <c r="C132" s="23"/>
+      <c r="D132" s="23"/>
+      <c r="E132" s="23"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
@@ -4941,12 +5177,12 @@
       <c r="P132" s="2"/>
       <c r="Q132" s="2"/>
     </row>
-    <row r="133" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
+    <row r="133" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="31"/>
+      <c r="B133" s="18"/>
+      <c r="C133" s="23"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="23"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
@@ -4960,12 +5196,12 @@
       <c r="P133" s="2"/>
       <c r="Q133" s="2"/>
     </row>
-    <row r="134" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
+    <row r="134" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="31"/>
+      <c r="B134" s="18"/>
+      <c r="C134" s="23"/>
+      <c r="D134" s="23"/>
+      <c r="E134" s="23"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
@@ -4979,12 +5215,12 @@
       <c r="P134" s="2"/>
       <c r="Q134" s="2"/>
     </row>
-    <row r="135" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
+    <row r="135" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="31"/>
+      <c r="B135" s="18"/>
+      <c r="C135" s="23"/>
+      <c r="D135" s="23"/>
+      <c r="E135" s="23"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
@@ -4998,12 +5234,12 @@
       <c r="P135" s="2"/>
       <c r="Q135" s="2"/>
     </row>
-    <row r="136" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
+    <row r="136" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="31"/>
+      <c r="B136" s="18"/>
+      <c r="C136" s="23"/>
+      <c r="D136" s="23"/>
+      <c r="E136" s="23"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
@@ -5017,12 +5253,12 @@
       <c r="P136" s="2"/>
       <c r="Q136" s="2"/>
     </row>
-    <row r="137" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
+    <row r="137" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="31"/>
+      <c r="B137" s="18"/>
+      <c r="C137" s="23"/>
+      <c r="D137" s="23"/>
+      <c r="E137" s="23"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
@@ -5036,12 +5272,12 @@
       <c r="P137" s="2"/>
       <c r="Q137" s="2"/>
     </row>
-    <row r="138" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
+    <row r="138" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="31"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
@@ -5055,12 +5291,12 @@
       <c r="P138" s="2"/>
       <c r="Q138" s="2"/>
     </row>
-    <row r="139" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
+    <row r="139" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="31"/>
+      <c r="B139" s="18"/>
+      <c r="C139" s="23"/>
+      <c r="D139" s="23"/>
+      <c r="E139" s="23"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
@@ -5074,12 +5310,12 @@
       <c r="P139" s="2"/>
       <c r="Q139" s="2"/>
     </row>
-    <row r="140" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
+    <row r="140" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="31"/>
+      <c r="B140" s="18"/>
+      <c r="C140" s="23"/>
+      <c r="D140" s="23"/>
+      <c r="E140" s="23"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
@@ -5093,12 +5329,12 @@
       <c r="P140" s="2"/>
       <c r="Q140" s="2"/>
     </row>
-    <row r="141" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
+    <row r="141" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="31"/>
+      <c r="B141" s="18"/>
+      <c r="C141" s="23"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="23"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
@@ -5112,12 +5348,12 @@
       <c r="P141" s="2"/>
       <c r="Q141" s="2"/>
     </row>
-    <row r="142" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
+    <row r="142" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="31"/>
+      <c r="B142" s="18"/>
+      <c r="C142" s="23"/>
+      <c r="D142" s="23"/>
+      <c r="E142" s="23"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
@@ -5131,12 +5367,12 @@
       <c r="P142" s="2"/>
       <c r="Q142" s="2"/>
     </row>
-    <row r="143" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
+    <row r="143" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="31"/>
+      <c r="B143" s="18"/>
+      <c r="C143" s="23"/>
+      <c r="D143" s="23"/>
+      <c r="E143" s="23"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
@@ -5150,12 +5386,12 @@
       <c r="P143" s="2"/>
       <c r="Q143" s="2"/>
     </row>
-    <row r="144" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
+    <row r="144" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="31"/>
+      <c r="B144" s="18"/>
+      <c r="C144" s="23"/>
+      <c r="D144" s="23"/>
+      <c r="E144" s="23"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
@@ -5169,12 +5405,12 @@
       <c r="P144" s="2"/>
       <c r="Q144" s="2"/>
     </row>
-    <row r="145" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
+    <row r="145" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="31"/>
+      <c r="B145" s="18"/>
+      <c r="C145" s="23"/>
+      <c r="D145" s="23"/>
+      <c r="E145" s="23"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
@@ -5188,12 +5424,12 @@
       <c r="P145" s="2"/>
       <c r="Q145" s="2"/>
     </row>
-    <row r="146" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
+    <row r="146" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="31"/>
+      <c r="B146" s="18"/>
+      <c r="C146" s="23"/>
+      <c r="D146" s="23"/>
+      <c r="E146" s="23"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
@@ -5207,12 +5443,12 @@
       <c r="P146" s="2"/>
       <c r="Q146" s="2"/>
     </row>
-    <row r="147" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
+    <row r="147" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="31"/>
+      <c r="B147" s="18"/>
+      <c r="C147" s="23"/>
+      <c r="D147" s="23"/>
+      <c r="E147" s="23"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -5226,12 +5462,12 @@
       <c r="P147" s="2"/>
       <c r="Q147" s="2"/>
     </row>
-    <row r="148" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
+    <row r="148" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="31"/>
+      <c r="B148" s="18"/>
+      <c r="C148" s="23"/>
+      <c r="D148" s="23"/>
+      <c r="E148" s="23"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
@@ -5245,12 +5481,12 @@
       <c r="P148" s="2"/>
       <c r="Q148" s="2"/>
     </row>
-    <row r="149" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
+    <row r="149" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="31"/>
+      <c r="B149" s="18"/>
+      <c r="C149" s="23"/>
+      <c r="D149" s="23"/>
+      <c r="E149" s="23"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -5264,12 +5500,12 @@
       <c r="P149" s="2"/>
       <c r="Q149" s="2"/>
     </row>
-    <row r="150" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
+    <row r="150" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="31"/>
+      <c r="B150" s="18"/>
+      <c r="C150" s="23"/>
+      <c r="D150" s="23"/>
+      <c r="E150" s="23"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
@@ -5283,12 +5519,12 @@
       <c r="P150" s="2"/>
       <c r="Q150" s="2"/>
     </row>
-    <row r="151" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
+    <row r="151" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="31"/>
+      <c r="B151" s="18"/>
+      <c r="C151" s="23"/>
+      <c r="D151" s="23"/>
+      <c r="E151" s="23"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
@@ -5302,12 +5538,12 @@
       <c r="P151" s="2"/>
       <c r="Q151" s="2"/>
     </row>
-    <row r="152" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
+    <row r="152" spans="1:17" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="31"/>
+      <c r="B152" s="18"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="23"/>
+      <c r="E152" s="23"/>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
@@ -5322,6 +5558,7 @@
       <c r="Q152" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -5331,53 +5568,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.46484375" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0.25</v>

</xml_diff>